<commit_message>
Update more leader loading info
</commit_message>
<xml_diff>
--- a/文档/文明和领袖.xlsx
+++ b/文档/文明和领袖.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C92593-8BC1-4538-A7A5-0759AF89C469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="27945" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +29,11 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="443">
   <si>
+    <t>蓝：已完成验证
+橙：技术验证失败，需要修改
+绿：已修改载入台词</t>
+  </si>
+  <si>
     <t>领袖特性</t>
   </si>
   <si>
@@ -108,6 +107,9 @@
   </si>
   <si>
     <t>阿拉伯</t>
+  </si>
+  <si>
+    <t>萨拉丁（维齐尔）</t>
   </si>
   <si>
     <t>信仰之正义</t>
@@ -336,6 +338,9 @@
     <t>蒙古治世</t>
   </si>
   <si>
+    <t>永乐皇帝</t>
+  </si>
+  <si>
     <t>里甲：10人以上的大城加成减半。</t>
   </si>
   <si>
@@ -360,6 +365,9 @@
     <t>克里</t>
   </si>
   <si>
+    <t>庞德梅克</t>
+  </si>
+  <si>
     <t>有利条款</t>
   </si>
   <si>
@@ -417,6 +425,9 @@
     <t>克里奥帕特拉（托勒密）</t>
   </si>
   <si>
+    <t>河神哈比降临：改名为“伊西斯女神降临”，两个皮肤的领袖特性互换</t>
+  </si>
+  <si>
     <t>王室土地</t>
   </si>
   <si>
@@ -432,7 +443,7 @@
     <t>你也配修奇观？</t>
   </si>
   <si>
-    <t>英国</t>
+    <t>英格兰</t>
   </si>
   <si>
     <t>维多利亚（帝国时代）</t>
@@ -456,6 +467,37 @@
     <t>维多利亚（蒸汽时代）</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>蒸汽时代：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI Emoji"/>
+        <charset val="134"/>
+      </rPr>
+      <t>🐎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不再提供+2生产力，工业区建筑提供5%而非10%。</t>
+    </r>
+  </si>
+  <si>
     <t>工业革命</t>
   </si>
   <si>
@@ -688,6 +730,9 @@
   </si>
   <si>
     <t>印加</t>
+  </si>
+  <si>
+    <t>帕查库特克</t>
   </si>
   <si>
     <t>安第斯路网（参照联合国叫法）</t>
@@ -845,6 +890,9 @@
     <t>朝鲜</t>
   </si>
   <si>
+    <t>善德</t>
+  </si>
+  <si>
     <t>花郎：有总督的城市+3科技，+3文化。</t>
   </si>
   <si>
@@ -860,6 +908,9 @@
     <t>主要是下面那位比她强</t>
   </si>
   <si>
+    <t>世宗</t>
+  </si>
+  <si>
     <t>谚文</t>
   </si>
   <si>
@@ -891,6 +942,9 @@
   </si>
   <si>
     <t>马里</t>
+  </si>
+  <si>
+    <t>曼萨·穆萨</t>
   </si>
   <si>
     <t>萨赫勒商人</t>
@@ -1147,6 +1201,9 @@
   </si>
   <si>
     <t>葡萄牙</t>
+  </si>
+  <si>
+    <t>若昂三世</t>
   </si>
   <si>
     <t>关闸</t>
@@ -1258,6 +1315,9 @@
     <t>斯基泰</t>
   </si>
   <si>
+    <t>托米丽司</t>
+  </si>
+  <si>
     <t>居鲁士杀手</t>
   </si>
   <si>
@@ -1321,6 +1381,9 @@
     <t>女王图书馆</t>
   </si>
   <si>
+    <t>诺贝尔奖：诺贝尔奖改为不需要议会同意即可开始，且周期变为20T。删去招募伟人获得的外交支持，改为大科大工点数+50%。</t>
+  </si>
+  <si>
     <t>UI：露天博物馆：忠诚度加成改为相邻单元格+1魅力</t>
   </si>
   <si>
@@ -1364,88 +1427,19 @@
   </si>
   <si>
     <t>UD：伊坎达</t>
-  </si>
-  <si>
-    <t>诺贝尔奖：诺贝尔奖改为不需要议会同意即可开始，且周期变为20T。删去招募伟人获得的外交支持，改为大科大工点数+50%。</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>河神哈比降临：改名为“伊西斯女神降临”，两个皮肤的领袖特性互换</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>蒸汽时代：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🐎</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不再提供+2生产力，工业区建筑提供5%而非10%。</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>曼萨·穆萨</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>帕查库特克</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>庞德梅克</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>若昂三世</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>托米丽司</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>善德</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>世宗</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>萨拉丁（维齐尔）</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝：已完成验证
-橙：技术验证失败，需要修改
-绿：已修改载入台词</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>永乐皇帝</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1475,41 +1469,168 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Segoe UI Emoji"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="Segoe UI Emoji"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1520,6 +1641,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1537,18 +1664,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1556,13 +1857,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1575,216 +2118,135 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -1795,7 +2257,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -1823,40 +2285,154 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2106,19 +2682,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.25" customWidth="1"/>
     <col min="2" max="2" width="30.375" customWidth="1"/>
@@ -2131,1743 +2707,1808 @@
     <col min="10" max="10" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="1" ht="40.5" spans="1:10">
       <c r="A1" s="3"/>
-      <c r="B1" s="21" t="s">
-        <v>441</v>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="54" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
+    </row>
+    <row r="2" ht="54" spans="1:9">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="14"/>
-      <c r="B3" s="18" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" ht="27" spans="1:10">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="14"/>
-      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="4" ht="27" spans="1:10">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>440</v>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A6" s="14"/>
-      <c r="B6" s="20" t="s">
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" ht="27" spans="1:10">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="8" ht="94.5" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="F8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" ht="27" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" ht="40.5" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="B10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="7" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="11" ht="27" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="F11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2"/>
+      <c r="B12" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+        <v>74</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="7" t="s">
         <v>82</v>
       </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="14"/>
+      <c r="F14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="2"/>
       <c r="J14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2"/>
+      <c r="B15" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2"/>
+      <c r="B16" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="14"/>
-      <c r="B17" s="22" t="s">
-        <v>442</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="2"/>
+      <c r="B17" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="14"/>
+        <v>98</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="2"/>
       <c r="J17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A18" s="14"/>
-      <c r="B18" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" ht="27" spans="1:10">
+      <c r="A18" s="2"/>
+      <c r="B18" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="14"/>
+        <v>102</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="2"/>
       <c r="J18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" ht="40.5" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>435</v>
+        <v>104</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="5" t="s">
-        <v>105</v>
+      <c r="H19" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="20" ht="40.5" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="5" t="s">
-        <v>111</v>
+      <c r="H20" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" ht="67.5" spans="1:10">
+      <c r="A21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I21" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="2"/>
       <c r="J21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>431</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" ht="27" spans="1:9">
+      <c r="A22" s="2"/>
+      <c r="B22" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="14"/>
-      <c r="B23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" ht="27" spans="1:10">
+      <c r="A23" s="2"/>
+      <c r="B23" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="14"/>
+        <v>129</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="2"/>
       <c r="J23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A25" s="14"/>
-      <c r="B25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>432</v>
+        <v>135</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" ht="30" spans="1:10">
+      <c r="A25" s="2"/>
+      <c r="B25" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
       <c r="J25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" ht="27" spans="1:10">
+      <c r="A26" s="2"/>
+      <c r="B26" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
+        <v>144</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
       <c r="J26" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="14"/>
-      <c r="B27" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="2"/>
+      <c r="B27" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>150</v>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="2"/>
+      <c r="B30" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="2"/>
       <c r="J30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" ht="21" customHeight="1" spans="1:9">
+      <c r="A31" s="2"/>
+      <c r="B31" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>167</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="33" ht="27" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>170</v>
+        <v>174</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>177</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>183</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="I34" s="14"/>
+        <v>184</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I34" s="2"/>
       <c r="J34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="2"/>
+      <c r="B35" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
+        <v>190</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
       <c r="J35" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" ht="40.5" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>194</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>191</v>
+        <v>196</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="5" t="s">
-        <v>192</v>
+      <c r="H36" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A37" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" ht="27" spans="1:9">
+      <c r="A37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="I37" s="14"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="2"/>
+      <c r="B38" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" ht="40.5" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>434</v>
+        <v>218</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="G40" s="2"/>
-      <c r="H40" s="4" t="s">
-        <v>216</v>
+      <c r="H40" s="6" t="s">
+        <v>223</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>219</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" ht="45.95" customHeight="1" spans="1:10">
+      <c r="A41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="I41" s="14"/>
+        <v>228</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" ht="65.1" customHeight="1" spans="1:9">
+      <c r="A42" s="2"/>
+      <c r="B42" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>234</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" ht="27" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>230</v>
+        <v>235</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="H43" s="5" t="s">
-        <v>233</v>
+      <c r="H43" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="I44" s="14"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="2"/>
+      <c r="B45" s="11" t="s">
+        <v>248</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" ht="54" x14ac:dyDescent="0.15">
+        <v>250</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" ht="54" spans="1:10">
       <c r="A46" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>246</v>
+        <v>251</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>248</v>
+        <v>254</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="G46" s="2"/>
-      <c r="H46" s="4" t="s">
-        <v>249</v>
+      <c r="H46" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="I47" s="14"/>
+        <v>261</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I47" s="2"/>
       <c r="J47" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" s="14"/>
-      <c r="B48" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="2"/>
+      <c r="B48" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
+        <v>267</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
       <c r="J48" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="14" t="s">
-        <v>262</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>438</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>263</v>
+        <v>270</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>271</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="I49" s="14"/>
+        <v>272</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="I49" s="2"/>
       <c r="J49" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="14"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="2"/>
       <c r="B50" s="13" t="s">
-        <v>439</v>
+        <v>276</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-    </row>
-    <row r="51" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>278</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" ht="27" spans="1:10">
       <c r="A51" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>274</v>
+        <v>282</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>433</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>288</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="I52" s="14"/>
-    </row>
-    <row r="53" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="14"/>
+        <v>290</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" ht="40.5" spans="1:10">
+      <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>284</v>
+        <v>293</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
+        <v>295</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
       <c r="J53" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="2" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="55" ht="27" spans="1:9">
       <c r="A55" s="2" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="56" ht="27" spans="1:9">
       <c r="A56" s="2" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" s="14" t="s">
-        <v>305</v>
+    <row r="57" spans="1:9">
+      <c r="A57" s="2" t="s">
+        <v>315</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="I57" s="14"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="14"/>
+        <v>318</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="14" t="s">
-        <v>312</v>
+        <v>95</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="I59" s="14"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" s="14"/>
+        <v>326</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
+        <v>331</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" ht="67.5" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>324</v>
+        <v>333</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="G61" s="2"/>
-      <c r="H61" s="5" t="s">
-        <v>327</v>
+      <c r="H61" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="14" t="s">
-        <v>329</v>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" ht="40.5" spans="1:9">
+      <c r="A62" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="I62" s="14"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" s="14"/>
+        <v>343</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>337</v>
+        <v>346</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>347</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
+        <v>348</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
       <c r="J63" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" s="14" t="s">
-        <v>340</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F64" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="I64" s="14"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="14"/>
+        <v>353</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-    </row>
-    <row r="66" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>358</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" ht="40.5" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>351</v>
+        <v>360</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>361</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>358</v>
+        <v>367</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>368</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="68" ht="27" spans="1:10">
       <c r="A68" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>436</v>
+        <v>373</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>374</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>368</v>
+        <v>378</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>379</v>
       </c>
       <c r="J68" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" s="14" t="s">
-        <v>370</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="I69" s="14"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" s="14"/>
+        <v>384</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-    </row>
-    <row r="71" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>389</v>
+      </c>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" ht="40.5" spans="1:10">
       <c r="A71" s="2" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>381</v>
+        <v>391</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>392</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="54" x14ac:dyDescent="0.15">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="72" ht="54" spans="1:10">
       <c r="A72" s="2" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>388</v>
+        <v>398</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>399</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>390</v>
+        <v>400</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>401</v>
       </c>
       <c r="G72" s="2"/>
-      <c r="H72" s="5" t="s">
-        <v>391</v>
+      <c r="H72" s="7" t="s">
+        <v>402</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>437</v>
+        <v>404</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>405</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="54" x14ac:dyDescent="0.15">
+    <row r="74" ht="54" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>402</v>
+        <v>413</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>414</v>
       </c>
       <c r="G74" s="2"/>
-      <c r="H74" s="4" t="s">
-        <v>403</v>
+      <c r="H74" s="6" t="s">
+        <v>415</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" ht="40.5" spans="1:9">
       <c r="A75" s="2" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="G75" s="2"/>
-      <c r="H75" s="8" t="s">
-        <v>409</v>
+      <c r="H75" s="15" t="s">
+        <v>421</v>
       </c>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="81" x14ac:dyDescent="0.15">
+    <row r="76" ht="81" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>430</v>
+        <v>426</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>427</v>
       </c>
       <c r="G76" s="2"/>
-      <c r="H76" s="5" t="s">
-        <v>415</v>
+      <c r="H76" s="7" t="s">
+        <v>428</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" ht="40.5" spans="1:10">
       <c r="A77" s="2" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>419</v>
+        <v>431</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>432</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>421</v>
+        <v>433</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>434</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="2" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="I78" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="H57:H58"/>
     <mergeCell ref="H59:H60"/>
     <mergeCell ref="H62:H63"/>
     <mergeCell ref="H64:H65"/>
@@ -3884,80 +4525,15 @@
     <mergeCell ref="I41:I42"/>
     <mergeCell ref="I44:I45"/>
     <mergeCell ref="I47:I48"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I69:I70"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dutch update and bugfixes
</commit_message>
<xml_diff>
--- a/文档/文明和领袖.xlsx
+++ b/文档/文明和领袖.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1485AC34-CE75-4E6A-A85D-D2E44D0EA4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86777DC0-5122-4B4B-B7D4-CCCDD212A822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="2445" windowWidth="24495" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1548,7 +1548,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1591,13 +1591,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1606,13 +1603,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2097,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2115,10 +2109,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>439</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2139,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="54" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2157,19 +2151,19 @@
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="15"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
@@ -2182,16 +2176,16 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
       <c r="J3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2201,16 +2195,16 @@
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
       <c r="J4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2222,17 +2216,17 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="7" t="s">
         <v>29</v>
       </c>
@@ -2242,10 +2236,10 @@
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="J6" t="s">
         <v>31</v>
       </c>
@@ -2352,7 +2346,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2367,20 +2361,20 @@
       <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="14"/>
       <c r="J11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>68</v>
       </c>
@@ -2390,10 +2384,10 @@
       <c r="D12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" t="s">
         <v>71</v>
       </c>
@@ -2424,7 +2418,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="18" t="s">
         <v>79</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2436,20 +2430,20 @@
       <c r="D14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="14"/>
       <c r="J14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>85</v>
       </c>
@@ -2459,13 +2453,13 @@
       <c r="D15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="16"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>88</v>
       </c>
@@ -2475,13 +2469,13 @@
       <c r="D16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="16"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>91</v>
       </c>
@@ -2491,16 +2485,16 @@
       <c r="D17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="14"/>
       <c r="J17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>95</v>
       </c>
@@ -2510,10 +2504,10 @@
       <c r="D18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="14"/>
       <c r="J18" t="s">
         <v>98</v>
       </c>
@@ -2544,7 +2538,7 @@
       <c r="A20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2566,10 +2560,10 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -2578,20 +2572,20 @@
       <c r="D21" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="18" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="14"/>
       <c r="J21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="4" t="s">
         <v>118</v>
       </c>
@@ -2601,14 +2595,14 @@
       <c r="D22" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
-      <c r="B23" s="20" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -2617,16 +2611,16 @@
       <c r="D23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="14"/>
       <c r="J23" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="18" t="s">
         <v>125</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2641,18 +2635,18 @@
       <c r="E24" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="I24" s="16"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A25" s="15"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -2661,17 +2655,17 @@
       <c r="D25" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
       <c r="J25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -2680,16 +2674,16 @@
       <c r="D26" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
       <c r="J26" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="15"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="4" t="s">
         <v>140</v>
       </c>
@@ -2699,10 +2693,10 @@
       <c r="D27" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
@@ -2727,7 +2721,7 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="14" t="s">
         <v>149</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2739,19 +2733,19 @@
       <c r="D29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="16"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
         <v>156</v>
       </c>
@@ -2761,17 +2755,17 @@
       <c r="D30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="16"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="14"/>
       <c r="J30" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="16"/>
-      <c r="B31" s="20" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2780,16 +2774,16 @@
       <c r="D31" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -2811,7 +2805,7 @@
       <c r="A33" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -2833,45 +2827,45 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="18" t="s">
         <v>175</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="13" t="s">
         <v>441</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16" t="s">
+      <c r="G34" s="14"/>
+      <c r="H34" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="I34" s="16"/>
+      <c r="I34" s="14"/>
       <c r="J34" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="15"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="2" t="s">
         <v>182</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
       <c r="J35" t="s">
         <v>184</v>
       </c>
@@ -2883,7 +2877,7 @@
       <c r="B36" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="13" t="s">
         <v>440</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2905,7 +2899,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="18" t="s">
         <v>192</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2917,17 +2911,17 @@
       <c r="D37" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16" t="s">
+      <c r="G37" s="14"/>
+      <c r="H37" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="I37" s="16"/>
+      <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="15"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="4" t="s">
         <v>198</v>
       </c>
@@ -2937,10 +2931,10 @@
       <c r="D38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
@@ -2999,7 +2993,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="14" t="s">
         <v>217</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -3011,20 +3005,20 @@
       <c r="D41" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="18" t="s">
+      <c r="G41" s="14"/>
+      <c r="H41" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I41" s="16"/>
+      <c r="I41" s="14"/>
       <c r="J41" s="2" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="4" t="s">
         <v>224</v>
       </c>
@@ -3034,16 +3028,16 @@
       <c r="D42" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="16"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="14"/>
     </row>
     <row r="43" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -3065,7 +3059,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="18" t="s">
         <v>234</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -3077,17 +3071,17 @@
       <c r="D44" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16" t="s">
+      <c r="G44" s="14"/>
+      <c r="H44" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="I44" s="16"/>
+      <c r="I44" s="14"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="15"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="4" t="s">
         <v>240</v>
       </c>
@@ -3097,16 +3091,16 @@
       <c r="D45" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="2" t="s">
         <v>244</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -3128,10 +3122,10 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="2" t="s">
         <v>251</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -3140,20 +3134,20 @@
       <c r="D47" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16" t="s">
+      <c r="G47" s="14"/>
+      <c r="H47" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="I47" s="16"/>
+      <c r="I47" s="14"/>
       <c r="J47" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" s="16"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="4" t="s">
         <v>257</v>
       </c>
@@ -3163,19 +3157,19 @@
       <c r="D48" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
       <c r="J48" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="2" t="s">
         <v>262</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -3184,20 +3178,20 @@
       <c r="D49" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16" t="s">
+      <c r="G49" s="14"/>
+      <c r="H49" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="I49" s="16"/>
+      <c r="I49" s="14"/>
       <c r="J49" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="15"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="4" t="s">
         <v>268</v>
       </c>
@@ -3207,16 +3201,16 @@
       <c r="D50" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
     </row>
     <row r="51" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="2" t="s">
         <v>272</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -3241,7 +3235,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="18" t="s">
         <v>279</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -3253,18 +3247,18 @@
       <c r="D52" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="F52" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16" t="s">
+      <c r="G52" s="14"/>
+      <c r="H52" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="I52" s="16"/>
+      <c r="I52" s="14"/>
     </row>
     <row r="53" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="15"/>
-      <c r="B53" s="20" t="s">
+      <c r="A53" s="18"/>
+      <c r="B53" s="2" t="s">
         <v>285</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -3273,10 +3267,10 @@
       <c r="D53" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
       <c r="J53" t="s">
         <v>288</v>
       </c>
@@ -3348,7 +3342,7 @@
       <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="18" t="s">
         <v>307</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -3360,17 +3354,17 @@
       <c r="D57" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="F57" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16" t="s">
+      <c r="G57" s="14"/>
+      <c r="H57" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="I57" s="16"/>
+      <c r="I57" s="14"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="15"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="4" t="s">
         <v>313</v>
       </c>
@@ -3380,13 +3374,13 @@
       <c r="D58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="18" t="s">
         <v>314</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -3401,17 +3395,17 @@
       <c r="E59" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16" t="s">
+      <c r="G59" s="14"/>
+      <c r="H59" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="I59" s="16"/>
+      <c r="I59" s="14"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="4" t="s">
         <v>321</v>
       </c>
@@ -3421,16 +3415,16 @@
       <c r="D60" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
     </row>
     <row r="61" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="2" t="s">
         <v>325</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -3452,7 +3446,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="18" t="s">
         <v>331</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3467,18 +3461,18 @@
       <c r="E62" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16" t="s">
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="I62" s="16"/>
+      <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" s="15"/>
-      <c r="B63" s="20" t="s">
+      <c r="A63" s="18"/>
+      <c r="B63" s="2" t="s">
         <v>338</v>
       </c>
       <c r="C63" s="6" t="s">
@@ -3487,16 +3481,16 @@
       <c r="D63" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
       <c r="J63" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="18" t="s">
         <v>342</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -3508,17 +3502,17 @@
       <c r="D64" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="F64" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16" t="s">
+      <c r="G64" s="14"/>
+      <c r="H64" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="I64" s="16"/>
+      <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="4" t="s">
         <v>348</v>
       </c>
@@ -3528,16 +3522,16 @@
       <c r="D65" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="2" t="s">
         <v>352</v>
       </c>
       <c r="C66" s="6" t="s">
@@ -3562,7 +3556,7 @@
       <c r="A67" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="2" t="s">
         <v>359</v>
       </c>
       <c r="C67" s="6" t="s">
@@ -3611,7 +3605,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="18" t="s">
         <v>373</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -3623,17 +3617,17 @@
       <c r="D69" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="F69" s="16" t="s">
+      <c r="F69" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16" t="s">
+      <c r="G69" s="14"/>
+      <c r="H69" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="I69" s="16"/>
+      <c r="I69" s="14"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" s="15"/>
+      <c r="A70" s="18"/>
       <c r="B70" s="4" t="s">
         <v>379</v>
       </c>
@@ -3643,16 +3637,16 @@
       <c r="D70" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
     </row>
     <row r="71" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="2" t="s">
         <v>383</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -3677,7 +3671,7 @@
       <c r="A72" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="2" t="s">
         <v>390</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -3799,7 +3793,7 @@
       <c r="A77" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="2" t="s">
         <v>423</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -3844,30 +3838,62 @@
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G62:G63"/>
     <mergeCell ref="G64:G65"/>
     <mergeCell ref="G69:G70"/>
     <mergeCell ref="H2:H4"/>
@@ -3884,62 +3910,30 @@
     <mergeCell ref="H47:H48"/>
     <mergeCell ref="H49:H50"/>
     <mergeCell ref="H52:H53"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I62:I63"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update Victoria age of steam
</commit_message>
<xml_diff>
--- a/文档/文明和领袖.xlsx
+++ b/文档/文明和领袖.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA053396-0B20-432D-AE3B-972A233BE869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4572EC9F-C898-48CD-A7B4-B26710DB56C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11595" yWindow="3870" windowWidth="24495" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2025" yWindow="5040" windowWidth="24495" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,37 +434,6 @@
     <t>维多利亚（蒸汽时代）</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>蒸汽时代：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🐎</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不再提供+2生产力，工业区建筑提供5%而非10%。</t>
-    </r>
-  </si>
-  <si>
     <t>工业革命</t>
   </si>
   <si>
@@ -1385,15 +1354,15 @@
   </si>
   <si>
     <t>特拉托阿尼</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>胜利者萨拉丁：陆地远程单位从每个相邻的友方单位获得2点远程战斗力</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>解放黑奴宣言</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1409,32 +1378,36 @@
       </rPr>
       <t>：相邻加成减半。</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>蓝：处理已完成
 橙：搁置中</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>可敬战役（1813年5月~8月的战役）</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>神圣罗马皇帝</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UI：圩田：额外1粮。+4金转为中世纪集市+2金</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>世界、王国与信仰的荣光：建造军事单位返还造价40%的信仰</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>索格伦之子：商业中心和市场各提供1大文点。著作加成改为+6金和+3产能。赞助伟人改为-50%成本。</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒸汽时代：战略资源的+2生产力需要改良，工业区建筑提供5%而非10%。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1464,12 +1437,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Segoe UI Emoji"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1486,6 +1453,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1550,7 +1525,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1587,19 +1562,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1608,10 +1580,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2096,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2114,10 +2092,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="B1" s="20"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2122,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="54" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2156,19 +2134,19 @@
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="15"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
@@ -2181,35 +2159,35 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
       <c r="J3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
       <c r="J4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2221,30 +2199,30 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="J6" t="s">
         <v>31</v>
       </c>
@@ -2282,7 +2260,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>41</v>
@@ -2351,7 +2329,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2366,20 +2344,20 @@
       <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="14"/>
       <c r="J11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>68</v>
       </c>
@@ -2389,10 +2367,10 @@
       <c r="D12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" t="s">
         <v>71</v>
       </c>
@@ -2423,7 +2401,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="18" t="s">
         <v>79</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2435,20 +2413,20 @@
       <c r="D14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19" t="s">
-        <v>436</v>
-      </c>
-      <c r="I14" s="16"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="I14" s="14"/>
       <c r="J14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>85</v>
       </c>
@@ -2458,13 +2436,13 @@
       <c r="D15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="16"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>88</v>
       </c>
@@ -2474,13 +2452,13 @@
       <c r="D16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="16"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>91</v>
       </c>
@@ -2490,16 +2468,16 @@
       <c r="D17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="14"/>
       <c r="J17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>95</v>
       </c>
@@ -2509,10 +2487,10 @@
       <c r="D18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="14"/>
       <c r="J18" t="s">
         <v>98</v>
       </c>
@@ -2557,7 +2535,7 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" t="s">
@@ -2565,7 +2543,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="18" t="s">
         <v>111</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2577,20 +2555,20 @@
       <c r="D21" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="18" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="14"/>
       <c r="J21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="4" t="s">
         <v>118</v>
       </c>
@@ -2600,13 +2578,13 @@
       <c r="D22" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="4" t="s">
         <v>121</v>
       </c>
@@ -2616,16 +2594,16 @@
       <c r="D23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="14"/>
       <c r="J23" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="18" t="s">
         <v>125</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2640,738 +2618,738 @@
       <c r="E24" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.15">
-      <c r="A25" s="15"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="18"/>
       <c r="B25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="21" t="s">
+        <v>442</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="A26" s="18"/>
+      <c r="B26" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="15"/>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="15"/>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="20" t="s">
+      <c r="B29" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="G29" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="H29" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" s="19"/>
+      <c r="B30" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="14"/>
+      <c r="J30" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="16"/>
-      <c r="J30" t="s">
+    </row>
+    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="19"/>
+      <c r="B31" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>161</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="16"/>
+        <v>137</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="18" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
+      <c r="B34" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="G34" s="14"/>
+      <c r="H34" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16" t="s">
+      <c r="I34" s="14"/>
+      <c r="J34" t="s">
         <v>178</v>
       </c>
-      <c r="I34" s="16"/>
-      <c r="J34" t="s">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="18"/>
+      <c r="B35" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="15"/>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" t="s">
         <v>182</v>
-      </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>438</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="A37" s="18" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A37" s="15" t="s">
+      <c r="B37" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="F37" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="G37" s="14"/>
+      <c r="H37" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16" t="s">
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="18"/>
+      <c r="B38" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I37" s="16"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="15"/>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="14" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="B41" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="F41" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="G41" s="14"/>
+      <c r="H41" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="18" t="s">
+      <c r="I41" s="14"/>
+      <c r="J41" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="14"/>
+      <c r="B42" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="16"/>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="16"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="14"/>
     </row>
     <row r="43" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="D43" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A44" s="18" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="15" t="s">
+      <c r="B44" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="G44" s="14"/>
+      <c r="H44" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16" t="s">
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A45" s="18"/>
+      <c r="B45" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I44" s="16"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="15"/>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A47" s="14" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="16" t="s">
+      <c r="B47" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="G47" s="14"/>
+      <c r="H47" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16" t="s">
+      <c r="I47" s="14"/>
+      <c r="J47" t="s">
         <v>254</v>
       </c>
-      <c r="I47" s="16"/>
-      <c r="J47" t="s">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A48" s="14"/>
+      <c r="B48" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" s="16"/>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="F48" s="16"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" t="s">
         <v>258</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" t="s">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A49" s="18" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="15" t="s">
+      <c r="B49" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="D49" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="F49" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="G49" s="14"/>
+      <c r="H49" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16" t="s">
+      <c r="I49" s="14"/>
+      <c r="J49" t="s">
         <v>265</v>
       </c>
-      <c r="I49" s="16"/>
-      <c r="J49" t="s">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A50" s="18"/>
+      <c r="B50" s="4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="15"/>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
     </row>
     <row r="51" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="F51" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A52" s="18" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
+      <c r="B52" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="F52" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="G52" s="14"/>
+      <c r="H52" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16" t="s">
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A53" s="18"/>
+      <c r="B53" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I52" s="16"/>
-    </row>
-    <row r="53" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="15"/>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" t="s">
         <v>285</v>
-      </c>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A57" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" s="15" t="s">
+      <c r="B57" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="F57" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="G57" s="14"/>
+      <c r="H57" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16" t="s">
+      <c r="I57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A58" s="18"/>
+      <c r="B58" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="I57" s="16"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="15"/>
-      <c r="B58" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>89</v>
@@ -3379,494 +3357,526 @@
       <c r="D58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="G59" s="14"/>
+      <c r="H59" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16" t="s">
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A60" s="18"/>
+      <c r="B60" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="I59" s="16"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" s="15"/>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
     </row>
     <row r="61" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="D61" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A62" s="18" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="15" t="s">
+      <c r="B62" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16" t="s">
+      <c r="I62" s="14"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A63" s="18"/>
+      <c r="B63" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="I62" s="16"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" s="15"/>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="D63" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" t="s">
         <v>338</v>
       </c>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" t="s">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A64" s="18" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" s="15" t="s">
+      <c r="B64" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="F64" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="G64" s="14"/>
+      <c r="H64" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16" t="s">
+      <c r="I64" s="14"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A65" s="18"/>
+      <c r="B65" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="I64" s="16"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="15"/>
-      <c r="B65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="D66" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="D67" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="I68" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="J68" t="s">
         <v>369</v>
       </c>
-      <c r="J68" t="s">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A69" s="18" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" s="15" t="s">
+      <c r="B69" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="F69" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="F69" s="16" t="s">
+      <c r="G69" s="14"/>
+      <c r="H69" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16" t="s">
+      <c r="I69" s="14"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A70" s="18"/>
+      <c r="B70" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="I69" s="16"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" s="15"/>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
     </row>
     <row r="71" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="D71" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="D72" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="F72" s="6" t="s">
         <v>390</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>391</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="F74" s="5" t="s">
         <v>403</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>404</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:10" ht="81" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="6" t="s">
         <v>416</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>417</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="D77" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="F77" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I78" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G62:G63"/>
     <mergeCell ref="G64:G65"/>
     <mergeCell ref="G69:G70"/>
     <mergeCell ref="H2:H4"/>
@@ -3883,64 +3893,32 @@
     <mergeCell ref="H47:H48"/>
     <mergeCell ref="H49:H50"/>
     <mergeCell ref="H52:H53"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I62:I63"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweaked Kurgan to avoid AI spamming it
</commit_message>
<xml_diff>
--- a/文档/文明和领袖.xlsx
+++ b/文档/文明和领袖.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19EE6E-8058-4F5E-9BFB-37AB76EAAC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14BFA92-42EF-45E5-ACF5-28A39FDBD044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2940" windowWidth="26205" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="4080" windowWidth="26205" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1257,9 +1257,6 @@
     <t>大草原之民</t>
   </si>
   <si>
-    <t>UI：库尔干坟冢</t>
-  </si>
-  <si>
     <t>西班牙</t>
   </si>
   <si>
@@ -1406,6 +1403,10 @@
   </si>
   <si>
     <t>胜利者萨拉丁</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI：库尔干坟冢:为避免AI爆出，只在与牧场相邻时+4金币</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1553,25 +1554,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2056,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2104,7 +2105,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="54" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2128,7 +2129,7 @@
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2150,7 +2151,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="19"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
@@ -2169,7 +2170,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2185,25 +2186,25 @@
         <v>29</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="18" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="19"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>442</v>
+      <c r="C6" s="12" t="s">
+        <v>441</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="13"/>
       <c r="J6" t="s">
         <v>33</v>
@@ -2245,7 +2246,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>44</v>
@@ -2291,7 +2292,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>56</v>
@@ -2311,7 +2312,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2326,7 +2327,7 @@
       <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>66</v>
       </c>
       <c r="G11" s="13"/>
@@ -2339,7 +2340,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="19"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
@@ -2349,7 +2350,7 @@
       <c r="D12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -2383,7 +2384,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2399,7 +2400,7 @@
         <v>84</v>
       </c>
       <c r="G14" s="13"/>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="19" t="s">
         <v>85</v>
       </c>
       <c r="I14" s="13"/>
@@ -2408,7 +2409,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="19"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="4" t="s">
         <v>87</v>
       </c>
@@ -2420,11 +2421,11 @@
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="15"/>
       <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="19"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>90</v>
       </c>
@@ -2436,11 +2437,11 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="16"/>
+      <c r="H16" s="15"/>
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="19"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>93</v>
       </c>
@@ -2452,14 +2453,14 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="15"/>
       <c r="I17" s="13"/>
       <c r="J17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A18" s="19"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="4" t="s">
         <v>97</v>
       </c>
@@ -2471,7 +2472,7 @@
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="13"/>
       <c r="J18" t="s">
         <v>100</v>
@@ -2525,14 +2526,14 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="14" t="s">
         <v>114</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>115</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>116</v>
@@ -2550,7 +2551,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2566,7 +2567,7 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>123</v>
       </c>
@@ -2585,7 +2586,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="14" t="s">
         <v>127</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2610,7 +2611,7 @@
       <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="4" t="s">
         <v>134</v>
       </c>
@@ -2629,7 +2630,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="4" t="s">
         <v>138</v>
       </c>
@@ -2648,7 +2649,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="4" t="s">
         <v>142</v>
       </c>
@@ -2686,7 +2687,7 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="14" t="s">
         <v>151</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2698,8 +2699,8 @@
       <c r="D29" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>434</v>
+      <c r="F29" s="16" t="s">
+        <v>433</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>155</v>
@@ -2710,7 +2711,7 @@
       <c r="I29" s="13"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="19"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
         <v>157</v>
       </c>
@@ -2729,7 +2730,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="19"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="4" t="s">
         <v>161</v>
       </c>
@@ -2792,7 +2793,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="14" t="s">
         <v>176</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -2817,7 +2818,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="19"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="4" t="s">
         <v>183</v>
       </c>
@@ -2864,7 +2865,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="27" x14ac:dyDescent="0.15">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="14" t="s">
         <v>195</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2886,7 +2887,7 @@
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="19"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="4" t="s">
         <v>201</v>
       </c>
@@ -2958,7 +2959,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="14" t="s">
         <v>220</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -2983,7 +2984,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="19"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="4" t="s">
         <v>227</v>
       </c>
@@ -3024,7 +3025,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="14" t="s">
         <v>237</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -3046,7 +3047,7 @@
       <c r="I44" s="13"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="19"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="4" t="s">
         <v>243</v>
       </c>
@@ -3087,7 +3088,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="14" t="s">
         <v>253</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3099,7 +3100,7 @@
       <c r="D47" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="F47" s="15" t="s">
         <v>257</v>
       </c>
       <c r="G47" s="13"/>
@@ -3112,7 +3113,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="4" t="s">
         <v>260</v>
       </c>
@@ -3122,7 +3123,7 @@
       <c r="D48" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F48" s="16"/>
+      <c r="F48" s="15"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
@@ -3131,7 +3132,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="14" t="s">
         <v>264</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -3156,7 +3157,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="19"/>
+      <c r="A50" s="14"/>
       <c r="B50" s="4" t="s">
         <v>271</v>
       </c>
@@ -3200,7 +3201,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="14" t="s">
         <v>282</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -3222,7 +3223,7 @@
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A53" s="19"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="4" t="s">
         <v>288</v>
       </c>
@@ -3307,7 +3308,7 @@
       <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="14" t="s">
         <v>310</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -3329,7 +3330,7 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="19"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="4" t="s">
         <v>316</v>
       </c>
@@ -3345,7 +3346,7 @@
       <c r="I58" s="13"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="14" t="s">
         <v>317</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -3370,7 +3371,7 @@
       <c r="I59" s="13"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" s="19"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="4" t="s">
         <v>324</v>
       </c>
@@ -3411,7 +3412,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="14" t="s">
         <v>334</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3436,7 +3437,7 @@
       <c r="I62" s="13"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" s="19"/>
+      <c r="A63" s="14"/>
       <c r="B63" s="4" t="s">
         <v>341</v>
       </c>
@@ -3455,7 +3456,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="14" t="s">
         <v>345</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -3477,7 +3478,7 @@
       <c r="I64" s="13"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="19"/>
+      <c r="A65" s="14"/>
       <c r="B65" s="4" t="s">
         <v>351</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>355</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>356</v>
@@ -3525,7 +3526,7 @@
         <v>361</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>362</v>
@@ -3570,7 +3571,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="14" t="s">
         <v>374</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -3592,7 +3593,7 @@
       <c r="I69" s="13"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" s="19"/>
+      <c r="A70" s="14"/>
       <c r="B70" s="4" t="s">
         <v>380</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>384</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>385</v>
@@ -3640,7 +3641,7 @@
         <v>390</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>391</v>
@@ -3657,7 +3658,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
         <v>395</v>
       </c>
@@ -3674,30 +3675,30 @@
         <v>399</v>
       </c>
       <c r="G73" s="2"/>
-      <c r="H73" s="2" t="s">
-        <v>400</v>
+      <c r="H73" s="20" t="s">
+        <v>442</v>
       </c>
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="F74" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>405</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" t="s">
@@ -3706,138 +3707,148 @@
     </row>
     <row r="75" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="E76" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="F76" s="10" t="s">
         <v>440</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>441</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A77" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="D77" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="F77" s="6" t="s">
         <v>422</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>423</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I78" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G62:G63"/>
     <mergeCell ref="F59:F60"/>
     <mergeCell ref="F62:F63"/>
     <mergeCell ref="F64:F65"/>
@@ -3854,51 +3865,41 @@
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="G47:G48"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>